<commit_message>
Updated semi final file
</commit_message>
<xml_diff>
--- a/Financial_Data/MoneyControl/Companies/IT Services & Consulting/Affle India Ltd/Pruned_Excel/Semi_Final/Affle India Ltd_Semi_Final.xlsx
+++ b/Financial_Data/MoneyControl/Companies/IT Services & Consulting/Affle India Ltd/Pruned_Excel/Semi_Final/Affle India Ltd_Semi_Final.xlsx
@@ -18,11 +18,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="101">
   <si>
     <t>Balance Sheet of Affle India(in Rs. Cr.)</t>
   </si>
   <si>
+    <t>Month</t>
+  </si>
+  <si>
     <t>Total share capital</t>
   </si>
   <si>
@@ -59,34 +62,37 @@
     <t>Total assets</t>
   </si>
   <si>
-    <t>Mar 15</t>
-  </si>
-  <si>
-    <t>Mar 16</t>
-  </si>
-  <si>
-    <t>Mar 17</t>
-  </si>
-  <si>
-    <t>Mar 18</t>
-  </si>
-  <si>
-    <t>Mar 19</t>
-  </si>
-  <si>
-    <t>Mar 20</t>
-  </si>
-  <si>
-    <t>Mar 21</t>
-  </si>
-  <si>
-    <t>Mar 22</t>
-  </si>
-  <si>
-    <t>Mar 23</t>
-  </si>
-  <si>
-    <t>Mar 24</t>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
+  <si>
+    <t>03</t>
   </si>
   <si>
     <t>Cash Flow of Affle India(in Rs. Cr.)</t>
@@ -185,9 +191,6 @@
     <t>Quarterly Results of Affle India(in Rs. Cr.)</t>
   </si>
   <si>
-    <t>Month</t>
-  </si>
-  <si>
     <t>Quarter</t>
   </si>
   <si>
@@ -245,34 +248,10 @@
     <t>Diluted eps.</t>
   </si>
   <si>
-    <t>2018</t>
-  </si>
-  <si>
-    <t>2019</t>
-  </si>
-  <si>
-    <t>2020</t>
-  </si>
-  <si>
-    <t>2021</t>
-  </si>
-  <si>
-    <t>2022</t>
-  </si>
-  <si>
-    <t>2023</t>
-  </si>
-  <si>
-    <t>2024</t>
-  </si>
-  <si>
     <t>09</t>
   </si>
   <si>
     <t>12</t>
-  </si>
-  <si>
-    <t>03</t>
   </si>
   <si>
     <t>06</t>
@@ -699,13 +678,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -745,414 +724,447 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2">
         <v>15.82</v>
-      </c>
-      <c r="C2">
-        <v>-7.67</v>
       </c>
       <c r="D2">
         <v>-7.67</v>
       </c>
       <c r="E2">
+        <v>-7.67</v>
+      </c>
+      <c r="F2">
         <v>8.16</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>3.13</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>20.34</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>28.87</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.13</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0.64</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>1.19</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>27.68</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>28.87</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
         <v>15.82</v>
-      </c>
-      <c r="C3">
-        <v>-2.66</v>
       </c>
       <c r="D3">
         <v>-2.66</v>
       </c>
       <c r="E3">
+        <v>-2.66</v>
+      </c>
+      <c r="F3">
         <v>13.17</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>5.09</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>24.44</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>42.44</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.17</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>5.54</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>9.199999999999999</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>33.24</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>42.44</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4">
         <v>24.29</v>
-      </c>
-      <c r="C4">
-        <v>-3.76</v>
       </c>
       <c r="D4">
         <v>-3.76</v>
       </c>
       <c r="E4">
+        <v>-3.76</v>
+      </c>
+      <c r="F4">
         <v>21.03</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>7.23</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>26.22</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>48.69</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.36</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>14.61</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>17.19</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>31.5</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>48.69</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5">
         <v>24.29</v>
-      </c>
-      <c r="C5">
-        <v>5.06</v>
       </c>
       <c r="D5">
         <v>5.06</v>
       </c>
       <c r="E5">
+        <v>5.06</v>
+      </c>
+      <c r="F5">
         <v>30.17</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>4.59</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>26.72</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>58.03</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.37</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>15.11</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>16.22</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>41.81</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>58.03</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6">
         <v>24.29</v>
-      </c>
-      <c r="C6">
-        <v>21.98</v>
       </c>
       <c r="D6">
         <v>21.98</v>
       </c>
       <c r="E6">
+        <v>21.98</v>
+      </c>
+      <c r="F6">
         <v>46.27</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>13</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>45.51</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>93.59</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.66</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>25.36</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>39.21</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>54.37</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>93.59</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
         <v>25.5</v>
-      </c>
-      <c r="C7">
-        <v>139.54</v>
       </c>
       <c r="D7">
         <v>139.54</v>
       </c>
       <c r="E7">
+        <v>139.54</v>
+      </c>
+      <c r="F7">
         <v>165.03</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>39.77</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>85.34</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>253.3</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>2.9</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>31.83</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>78.08</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>175.22</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>253.3</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8">
         <v>25.5</v>
-      </c>
-      <c r="C8">
-        <v>167.69</v>
       </c>
       <c r="D8">
         <v>167.69</v>
       </c>
       <c r="E8">
+        <v>167.69</v>
+      </c>
+      <c r="F8">
         <v>193.19</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>14.4</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>87.72</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>302.77</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>2.34</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>33.49</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>162.1</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>140.68</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>302.77</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9">
         <v>26.65</v>
-      </c>
-      <c r="C9">
-        <v>817.11</v>
       </c>
       <c r="D9">
         <v>817.11</v>
       </c>
       <c r="E9">
+        <v>817.11</v>
+      </c>
+      <c r="F9">
         <v>843.76</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>18.6</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>168.59</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>1017.86</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>1.43</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>30.97</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>387.12</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>630.74</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>1017.86</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
         <v>26.64</v>
-      </c>
-      <c r="C10">
-        <v>882.4400000000001</v>
       </c>
       <c r="D10">
         <v>882.4400000000001</v>
       </c>
       <c r="E10">
+        <v>882.4400000000001</v>
+      </c>
+      <c r="F10">
         <v>909.0700000000001</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>16.47</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>191.2</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>1105.45</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>1.8</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>30.64</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>325.11</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>780.34</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>1105.45</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11">
         <v>28.02</v>
-      </c>
-      <c r="C11">
-        <v>1703.11</v>
       </c>
       <c r="D11">
         <v>1703.11</v>
       </c>
       <c r="E11">
+        <v>1703.11</v>
+      </c>
+      <c r="F11">
         <v>1731.13</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>28.99</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>288.38</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>2027.2</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>5.73</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>34.41</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>748.8</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>1278.4</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>2027.2</v>
       </c>
     </row>
@@ -1163,328 +1175,361 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2">
+        <v>1.73</v>
+      </c>
+      <c r="D2">
+        <v>0.43</v>
+      </c>
+      <c r="E2">
+        <v>0.51</v>
+      </c>
+      <c r="F2">
+        <v>-0.12</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0.82</v>
+      </c>
+      <c r="I2">
+        <v>0.77</v>
+      </c>
+      <c r="J2">
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>4.86</v>
+      </c>
+      <c r="D3">
+        <v>5.82</v>
+      </c>
+      <c r="E3">
+        <v>-7.81</v>
+      </c>
+      <c r="F3">
+        <v>7.22</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>5.24</v>
+      </c>
+      <c r="I3">
+        <v>1.59</v>
+      </c>
+      <c r="J3">
+        <v>6.83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <v>0.8</v>
+      </c>
+      <c r="D4">
+        <v>5.83</v>
+      </c>
+      <c r="E4">
+        <v>-5.7</v>
+      </c>
+      <c r="F4">
+        <v>-2.21</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>-2.08</v>
+      </c>
+      <c r="I4">
+        <v>7.87</v>
+      </c>
+      <c r="J4">
+        <v>5.79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <v>13.6</v>
+      </c>
+      <c r="D5">
+        <v>17.4</v>
+      </c>
+      <c r="E5">
+        <v>-1.4</v>
+      </c>
+      <c r="F5">
+        <v>-8.119999999999999</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>7.88</v>
+      </c>
+      <c r="I5">
+        <v>5.79</v>
+      </c>
+      <c r="J5">
+        <v>13.67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>23.54</v>
+      </c>
+      <c r="D6">
+        <v>17.53</v>
+      </c>
+      <c r="E6">
+        <v>-22.29</v>
+      </c>
+      <c r="F6">
+        <v>-0.43</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>-5.18</v>
+      </c>
+      <c r="I6">
+        <v>13.67</v>
+      </c>
+      <c r="J6">
+        <v>8.49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>44.03</v>
+      </c>
+      <c r="D7">
+        <v>32.01</v>
+      </c>
+      <c r="E7">
+        <v>-68.41</v>
+      </c>
+      <c r="F7">
+        <v>85.19</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>48.79</v>
+      </c>
+      <c r="I7">
+        <v>8.49</v>
+      </c>
+      <c r="J7">
+        <v>57.28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>39.57</v>
+      </c>
+      <c r="D8">
+        <v>15.25</v>
+      </c>
+      <c r="E8">
+        <v>-51.59</v>
+      </c>
+      <c r="F8">
+        <v>-0.74</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>-37.08</v>
+      </c>
+      <c r="I8">
+        <v>57.28</v>
+      </c>
+      <c r="J8">
+        <v>20.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9">
+        <v>75.81999999999999</v>
+      </c>
+      <c r="D9">
+        <v>58.78</v>
+      </c>
+      <c r="E9">
+        <v>-472.81</v>
+      </c>
+      <c r="F9">
+        <v>590.38</v>
+      </c>
+      <c r="G9">
+        <v>-0.01</v>
+      </c>
+      <c r="H9">
+        <v>176.34</v>
+      </c>
+      <c r="I9">
+        <v>20.2</v>
+      </c>
+      <c r="J9">
+        <v>196.54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>90.04000000000001</v>
+      </c>
+      <c r="D10">
+        <v>59.35</v>
+      </c>
+      <c r="E10">
+        <v>-79.39</v>
+      </c>
+      <c r="F10">
+        <v>-8.25</v>
+      </c>
+      <c r="G10">
+        <v>0.17</v>
+      </c>
+      <c r="H10">
+        <v>-27.18</v>
+      </c>
+      <c r="I10">
+        <v>196.54</v>
+      </c>
+      <c r="J10">
+        <v>169.35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B11" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2">
-        <v>1.73</v>
-      </c>
-      <c r="C2">
-        <v>0.43</v>
-      </c>
-      <c r="D2">
-        <v>0.51</v>
-      </c>
-      <c r="E2">
-        <v>-0.12</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0.82</v>
-      </c>
-      <c r="H2">
-        <v>0.77</v>
-      </c>
-      <c r="I2">
-        <v>1.59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3">
-        <v>4.86</v>
-      </c>
-      <c r="C3">
-        <v>5.82</v>
-      </c>
-      <c r="D3">
-        <v>-7.81</v>
-      </c>
-      <c r="E3">
-        <v>7.22</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>5.24</v>
-      </c>
-      <c r="H3">
-        <v>1.59</v>
-      </c>
-      <c r="I3">
-        <v>6.83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4">
-        <v>0.8</v>
-      </c>
-      <c r="C4">
-        <v>5.83</v>
-      </c>
-      <c r="D4">
-        <v>-5.7</v>
-      </c>
-      <c r="E4">
-        <v>-2.21</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>-2.08</v>
-      </c>
-      <c r="H4">
-        <v>7.87</v>
-      </c>
-      <c r="I4">
-        <v>5.79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5">
-        <v>13.6</v>
-      </c>
-      <c r="C5">
-        <v>17.4</v>
-      </c>
-      <c r="D5">
-        <v>-1.4</v>
-      </c>
-      <c r="E5">
-        <v>-8.119999999999999</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>7.88</v>
-      </c>
-      <c r="H5">
-        <v>5.79</v>
-      </c>
-      <c r="I5">
-        <v>13.67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
-        <v>23.54</v>
-      </c>
-      <c r="C6">
-        <v>17.53</v>
-      </c>
-      <c r="D6">
-        <v>-22.29</v>
-      </c>
-      <c r="E6">
-        <v>-0.43</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>-5.18</v>
-      </c>
-      <c r="H6">
-        <v>13.67</v>
-      </c>
-      <c r="I6">
-        <v>8.49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7">
-        <v>44.03</v>
-      </c>
-      <c r="C7">
-        <v>32.01</v>
-      </c>
-      <c r="D7">
-        <v>-68.41</v>
-      </c>
-      <c r="E7">
-        <v>85.19</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>48.79</v>
-      </c>
-      <c r="H7">
-        <v>8.49</v>
-      </c>
-      <c r="I7">
-        <v>57.28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8">
-        <v>39.57</v>
-      </c>
-      <c r="C8">
-        <v>15.25</v>
-      </c>
-      <c r="D8">
-        <v>-51.59</v>
-      </c>
-      <c r="E8">
-        <v>-0.74</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>-37.08</v>
-      </c>
-      <c r="H8">
-        <v>57.28</v>
-      </c>
-      <c r="I8">
-        <v>20.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9">
-        <v>75.81999999999999</v>
-      </c>
-      <c r="C9">
-        <v>58.78</v>
-      </c>
-      <c r="D9">
-        <v>-472.81</v>
-      </c>
-      <c r="E9">
-        <v>590.38</v>
-      </c>
-      <c r="F9">
-        <v>-0.01</v>
-      </c>
-      <c r="G9">
-        <v>176.34</v>
-      </c>
-      <c r="H9">
-        <v>20.2</v>
-      </c>
-      <c r="I9">
-        <v>196.54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10">
-        <v>90.04000000000001</v>
-      </c>
-      <c r="C10">
-        <v>59.35</v>
-      </c>
-      <c r="D10">
-        <v>-79.39</v>
-      </c>
-      <c r="E10">
-        <v>-8.25</v>
-      </c>
-      <c r="F10">
-        <v>0.17</v>
-      </c>
-      <c r="G10">
-        <v>-27.18</v>
-      </c>
-      <c r="H10">
-        <v>196.54</v>
-      </c>
-      <c r="I10">
+      <c r="C11">
+        <v>101.65</v>
+      </c>
+      <c r="D11">
+        <v>8.24</v>
+      </c>
+      <c r="E11">
+        <v>-689.63</v>
+      </c>
+      <c r="F11">
+        <v>739.88</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>58.48</v>
+      </c>
+      <c r="I11">
         <v>169.35</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11">
-        <v>101.65</v>
-      </c>
-      <c r="C11">
-        <v>8.24</v>
-      </c>
-      <c r="D11">
-        <v>-689.63</v>
-      </c>
-      <c r="E11">
-        <v>739.88</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>58.48</v>
-      </c>
-      <c r="H11">
-        <v>169.35</v>
-      </c>
-      <c r="I11">
+      <c r="J11">
         <v>227.83</v>
       </c>
     </row>
@@ -1495,86 +1540,89 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V11"/>
+  <dimension ref="A1:W11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22">
+        <v>54</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
       <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2">
-        <v>39.33</v>
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
       </c>
       <c r="C2">
         <v>39.33</v>
@@ -1583,46 +1631,46 @@
         <v>39.33</v>
       </c>
       <c r="E2">
+        <v>39.33</v>
+      </c>
+      <c r="F2">
         <v>0.13</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>39.46</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>28.18</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>5.36</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.15</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0.11</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>3.94</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>37.73</v>
-      </c>
-      <c r="M2">
-        <v>1.73</v>
       </c>
       <c r="N2">
         <v>1.73</v>
       </c>
       <c r="O2">
+        <v>1.73</v>
+      </c>
+      <c r="P2">
         <v>0.12</v>
-      </c>
-      <c r="P2">
-        <v>-0.53</v>
       </c>
       <c r="Q2">
         <v>-0.53</v>
       </c>
       <c r="R2">
-        <v>2.25</v>
+        <v>-0.53</v>
       </c>
       <c r="S2">
         <v>2.25</v>
@@ -1631,18 +1679,21 @@
         <v>2.25</v>
       </c>
       <c r="U2">
-        <v>1.43</v>
+        <v>2.25</v>
       </c>
       <c r="V2">
         <v>1.43</v>
       </c>
-    </row>
-    <row r="3" spans="1:22">
+      <c r="W2">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3">
-        <v>72.43000000000001</v>
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
       </c>
       <c r="C3">
         <v>72.43000000000001</v>
@@ -1651,46 +1702,46 @@
         <v>72.43000000000001</v>
       </c>
       <c r="E3">
+        <v>72.43000000000001</v>
+      </c>
+      <c r="F3">
         <v>0.27</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>72.7</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>51.84</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>7.08</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.87</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>0.26</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>7.8</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>67.84999999999999</v>
-      </c>
-      <c r="M3">
-        <v>4.86</v>
       </c>
       <c r="N3">
         <v>4.86</v>
       </c>
       <c r="O3">
+        <v>4.86</v>
+      </c>
+      <c r="P3">
         <v>0.8100000000000001</v>
-      </c>
-      <c r="P3">
-        <v>-0.15</v>
       </c>
       <c r="Q3">
         <v>-0.15</v>
       </c>
       <c r="R3">
-        <v>5.01</v>
+        <v>-0.15</v>
       </c>
       <c r="S3">
         <v>5.01</v>
@@ -1699,18 +1750,21 @@
         <v>5.01</v>
       </c>
       <c r="U3">
-        <v>3.16</v>
+        <v>5.01</v>
       </c>
       <c r="V3">
         <v>3.16</v>
       </c>
-    </row>
-    <row r="4" spans="1:22">
+      <c r="W3">
+        <v>3.16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4">
-        <v>65.63</v>
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
       </c>
       <c r="C4">
         <v>65.63</v>
@@ -1719,46 +1773,46 @@
         <v>65.63</v>
       </c>
       <c r="E4">
+        <v>65.63</v>
+      </c>
+      <c r="F4">
         <v>1.17</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>66.8</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>32.38</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>17.62</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>1.59</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>2.31</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>12.11</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>66</v>
-      </c>
-      <c r="M4">
-        <v>0.8</v>
       </c>
       <c r="N4">
         <v>0.8</v>
       </c>
       <c r="O4">
+        <v>0.8</v>
+      </c>
+      <c r="P4">
         <v>0.18</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>0.29</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>0.47</v>
-      </c>
-      <c r="R4">
-        <v>0.33</v>
       </c>
       <c r="S4">
         <v>0.33</v>
@@ -1767,18 +1821,21 @@
         <v>0.33</v>
       </c>
       <c r="U4">
-        <v>0.14</v>
+        <v>0.33</v>
       </c>
       <c r="V4">
         <v>0.14</v>
       </c>
-    </row>
-    <row r="5" spans="1:22">
+      <c r="W4">
+        <v>0.14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5">
-        <v>83.76000000000001</v>
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
       </c>
       <c r="C5">
         <v>83.76000000000001</v>
@@ -1787,46 +1844,46 @@
         <v>83.76000000000001</v>
       </c>
       <c r="E5">
+        <v>83.76000000000001</v>
+      </c>
+      <c r="F5">
         <v>1.12</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>84.88</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>42.43</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>15.95</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>1.08</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>3.21</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>8.609999999999999</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>71.28</v>
-      </c>
-      <c r="M5">
-        <v>13.6</v>
       </c>
       <c r="N5">
         <v>13.6</v>
       </c>
       <c r="O5">
+        <v>13.6</v>
+      </c>
+      <c r="P5">
         <v>4.62</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>0.15</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>4.77</v>
-      </c>
-      <c r="R5">
-        <v>8.83</v>
       </c>
       <c r="S5">
         <v>8.83</v>
@@ -1835,18 +1892,21 @@
         <v>8.83</v>
       </c>
       <c r="U5">
-        <v>3.64</v>
+        <v>8.83</v>
       </c>
       <c r="V5">
         <v>3.64</v>
       </c>
-    </row>
-    <row r="6" spans="1:22">
+      <c r="W5">
+        <v>3.64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
-        <v>121.21</v>
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
       </c>
       <c r="C6">
         <v>121.21</v>
@@ -1855,46 +1915,46 @@
         <v>121.21</v>
       </c>
       <c r="E6">
+        <v>121.21</v>
+      </c>
+      <c r="F6">
         <v>0.23</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>121.45</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>62.29</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>19.55</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.45</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>4.41</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>11.21</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>97.90000000000001</v>
-      </c>
-      <c r="M6">
-        <v>23.54</v>
       </c>
       <c r="N6">
         <v>23.54</v>
       </c>
       <c r="O6">
+        <v>23.54</v>
+      </c>
+      <c r="P6">
         <v>6.1</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>0.77</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>6.86</v>
-      </c>
-      <c r="R6">
-        <v>16.68</v>
       </c>
       <c r="S6">
         <v>16.68</v>
@@ -1903,66 +1963,69 @@
         <v>16.68</v>
       </c>
       <c r="U6">
-        <v>6.87</v>
+        <v>16.68</v>
       </c>
       <c r="V6">
         <v>6.87</v>
       </c>
-    </row>
-    <row r="7" spans="1:22">
+      <c r="W6">
+        <v>6.87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7">
-        <v>176.07</v>
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
       </c>
       <c r="C7">
         <v>176.07</v>
       </c>
       <c r="D7">
+        <v>176.07</v>
+      </c>
+      <c r="E7">
         <v>182.23</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>5.13</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>187.36</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>97.64</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>24.17</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>0.31</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>5.41</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>15.8</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>143.33</v>
-      </c>
-      <c r="M7">
-        <v>44.03</v>
       </c>
       <c r="N7">
         <v>44.03</v>
       </c>
       <c r="O7">
+        <v>44.03</v>
+      </c>
+      <c r="P7">
         <v>11.26</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>-0.12</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>11.14</v>
-      </c>
-      <c r="R7">
-        <v>32.89</v>
       </c>
       <c r="S7">
         <v>32.89</v>
@@ -1971,66 +2034,69 @@
         <v>32.89</v>
       </c>
       <c r="U7">
-        <v>13.12</v>
+        <v>32.89</v>
       </c>
       <c r="V7">
         <v>13.12</v>
       </c>
-    </row>
-    <row r="8" spans="1:22">
+      <c r="W7">
+        <v>13.12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8">
-        <v>258.95</v>
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
       </c>
       <c r="C8">
         <v>258.95</v>
       </c>
       <c r="D8">
+        <v>258.95</v>
+      </c>
+      <c r="E8">
         <v>266.73</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>6.45</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>273.18</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>159.36</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>31.78</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>0.36</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>6.57</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>35.54</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>233.61</v>
-      </c>
-      <c r="M8">
-        <v>39.57</v>
       </c>
       <c r="N8">
         <v>39.57</v>
       </c>
       <c r="O8">
+        <v>39.57</v>
+      </c>
+      <c r="P8">
         <v>9.15</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>2.19</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>11.34</v>
-      </c>
-      <c r="R8">
-        <v>28.23</v>
       </c>
       <c r="S8">
         <v>28.23</v>
@@ -2039,66 +2105,69 @@
         <v>28.23</v>
       </c>
       <c r="U8">
-        <v>11.07</v>
+        <v>28.23</v>
       </c>
       <c r="V8">
         <v>11.07</v>
       </c>
-    </row>
-    <row r="9" spans="1:22">
+      <c r="W8">
+        <v>11.07</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
       <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9">
-        <v>384.4</v>
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
       </c>
       <c r="C9">
         <v>384.4</v>
       </c>
       <c r="D9">
+        <v>384.4</v>
+      </c>
+      <c r="E9">
         <v>397.52</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>31.18</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>428.7</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>245.79</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>44.16</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0.65</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>7.29</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>55</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>352.88</v>
-      </c>
-      <c r="M9">
-        <v>75.81999999999999</v>
       </c>
       <c r="N9">
         <v>75.81999999999999</v>
       </c>
       <c r="O9">
+        <v>75.81999999999999</v>
+      </c>
+      <c r="P9">
         <v>18.05</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>1.3</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>19.27</v>
-      </c>
-      <c r="R9">
-        <v>56.55</v>
       </c>
       <c r="S9">
         <v>56.55</v>
@@ -2107,66 +2176,69 @@
         <v>56.55</v>
       </c>
       <c r="U9">
-        <v>4.26</v>
+        <v>56.55</v>
       </c>
       <c r="V9">
         <v>4.26</v>
       </c>
-    </row>
-    <row r="10" spans="1:22">
+      <c r="W9">
+        <v>4.26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10">
-        <v>476.94</v>
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
       </c>
       <c r="C10">
         <v>476.94</v>
       </c>
       <c r="D10">
+        <v>476.94</v>
+      </c>
+      <c r="E10">
         <v>494.8</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>22.57</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>517.37</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>307.16</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>46.94</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0.2</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>7.44</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>65.59</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>427.33</v>
-      </c>
-      <c r="M10">
-        <v>90.04000000000001</v>
       </c>
       <c r="N10">
         <v>90.04000000000001</v>
       </c>
       <c r="O10">
+        <v>90.04000000000001</v>
+      </c>
+      <c r="P10">
         <v>23.75</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>-0.59</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>23.16</v>
-      </c>
-      <c r="R10">
-        <v>66.88</v>
       </c>
       <c r="S10">
         <v>66.88</v>
@@ -2175,66 +2247,69 @@
         <v>66.88</v>
       </c>
       <c r="U10">
-        <v>5.02</v>
+        <v>66.88</v>
       </c>
       <c r="V10">
         <v>5.02</v>
       </c>
-    </row>
-    <row r="11" spans="1:22">
+      <c r="W10">
+        <v>5.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11">
-        <v>545.1799999999999</v>
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
       </c>
       <c r="C11">
         <v>545.1799999999999</v>
       </c>
       <c r="D11">
+        <v>545.1799999999999</v>
+      </c>
+      <c r="E11">
         <v>565.99</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>36.32</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>602.3099999999999</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>365.54</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>51.04</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>0.67</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>8.109999999999999</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>75.3</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>500.66</v>
-      </c>
-      <c r="M11">
-        <v>101.65</v>
       </c>
       <c r="N11">
         <v>101.65</v>
       </c>
       <c r="O11">
+        <v>101.65</v>
+      </c>
+      <c r="P11">
         <v>26.14</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>-0.45</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>25.7</v>
-      </c>
-      <c r="R11">
-        <v>75.95999999999999</v>
       </c>
       <c r="S11">
         <v>75.95999999999999</v>
@@ -2243,9 +2318,12 @@
         <v>75.95999999999999</v>
       </c>
       <c r="U11">
+        <v>75.95999999999999</v>
+      </c>
+      <c r="V11">
         <v>5.6</v>
       </c>
-      <c r="V11">
+      <c r="W11">
         <v>5.6</v>
       </c>
     </row>
@@ -2264,84 +2342,84 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D2">
         <v>27.53</v>
@@ -2406,13 +2484,13 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D3">
         <v>34.74</v>
@@ -2477,13 +2555,13 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D4">
         <v>29.84</v>
@@ -2548,13 +2626,13 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D5">
         <v>30.41</v>
@@ -2619,13 +2697,13 @@
     </row>
     <row r="6" spans="1:23">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
         <v>76</v>
       </c>
-      <c r="B6" t="s">
-        <v>82</v>
-      </c>
       <c r="C6" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D6">
         <v>49.23</v>
@@ -2690,13 +2768,13 @@
     </row>
     <row r="7" spans="1:23">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D7">
         <v>53.04</v>
@@ -2761,13 +2839,13 @@
     </row>
     <row r="8" spans="1:23">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D8">
         <v>43.39</v>
@@ -2832,13 +2910,13 @@
     </row>
     <row r="9" spans="1:23">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D9">
         <v>42.26</v>
@@ -2903,13 +2981,13 @@
     </row>
     <row r="10" spans="1:23">
       <c r="A10" t="s">
-        <v>77</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D10">
         <v>72.65000000000001</v>
@@ -2974,13 +3052,13 @@
     </row>
     <row r="11" spans="1:23">
       <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
         <v>77</v>
       </c>
-      <c r="B11" t="s">
-        <v>83</v>
-      </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D11">
         <v>78.31999999999999</v>
@@ -3045,13 +3123,13 @@
     </row>
     <row r="12" spans="1:23">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D12">
         <v>72.23</v>
@@ -3116,13 +3194,13 @@
     </row>
     <row r="13" spans="1:23">
       <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
         <v>78</v>
       </c>
-      <c r="B13" t="s">
-        <v>85</v>
-      </c>
       <c r="C13" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D13">
         <v>81.84999999999999</v>
@@ -3187,13 +3265,13 @@
     </row>
     <row r="14" spans="1:23">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D14">
         <v>95.97</v>
@@ -3258,13 +3336,13 @@
     </row>
     <row r="15" spans="1:23">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D15">
         <v>111.27</v>
@@ -3329,13 +3407,13 @@
     </row>
     <row r="16" spans="1:23">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D16">
         <v>108.44</v>
@@ -3400,13 +3478,13 @@
     </row>
     <row r="17" spans="1:23">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D17">
         <v>105.16</v>
@@ -3471,13 +3549,13 @@
     </row>
     <row r="18" spans="1:23">
       <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" t="s">
         <v>79</v>
-      </c>
-      <c r="B18" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" t="s">
-        <v>86</v>
       </c>
       <c r="D18">
         <v>115.86</v>
@@ -3542,13 +3620,13 @@
     </row>
     <row r="19" spans="1:23">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D19">
         <v>137.27</v>
@@ -3613,13 +3691,13 @@
     </row>
     <row r="20" spans="1:23">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D20">
         <v>136.5</v>
@@ -3684,13 +3762,13 @@
     </row>
     <row r="21" spans="1:23">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D21">
         <v>137.13</v>
@@ -3755,13 +3833,13 @@
     </row>
     <row r="22" spans="1:23">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C22" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D22">
         <v>133.83</v>
@@ -3826,13 +3904,13 @@
     </row>
     <row r="23" spans="1:23">
       <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" t="s">
         <v>80</v>
-      </c>
-      <c r="B23" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" t="s">
-        <v>87</v>
       </c>
       <c r="D23">
         <v>139.32</v>
@@ -3897,13 +3975,13 @@
     </row>
     <row r="24" spans="1:23">
       <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
         <v>81</v>
-      </c>
-      <c r="B24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24" t="s">
-        <v>88</v>
       </c>
       <c r="D24">
         <v>155.72</v>
@@ -3968,13 +4046,13 @@
     </row>
     <row r="25" spans="1:23">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D25">
         <v>163.15</v>
@@ -4039,13 +4117,13 @@
     </row>
     <row r="26" spans="1:23">
       <c r="A26" t="s">
-        <v>81</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D26">
         <v>176.1</v>
@@ -4115,108 +4193,111 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2">
         <v>24.85</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>1.25</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1.18</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1.09</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>1.42</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>5.03</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>4.76</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>4.39</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>5.73</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>27.62</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>7.8</v>
       </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
       <c r="N2">
         <v>0</v>
       </c>
@@ -4232,50 +4313,53 @@
       <c r="R2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:18">
+      <c r="S2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
         <v>45.77</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>3.78</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>3.62</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>3.07</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>3.16</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>8.25</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>7.9</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>6.7</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>6.91</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>38.03</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>11.8</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>0.33</v>
       </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
       <c r="O3">
         <v>0</v>
       </c>
@@ -4288,50 +4372,53 @@
       <c r="R3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:18">
+      <c r="S3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4">
         <v>27.02</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>1.93</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0.98</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>0.33</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.14</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>7.15</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>3.63</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>1.21</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>0.5</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>1.56</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>0.67</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>0.16</v>
       </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
       <c r="O4">
         <v>0</v>
       </c>
@@ -4344,47 +4431,50 @@
       <c r="R4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:18">
+      <c r="S4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5">
         <v>34.48</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>7.36</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>6.04</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>5.6</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>3.64</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>21.35</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>17.51</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>16.23</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>10.54</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>29.27</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>15.21</v>
       </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
       <c r="N5">
         <v>0</v>
       </c>
@@ -4400,47 +4490,50 @@
       <c r="R5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:18">
+      <c r="S5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6">
         <v>49.91</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>11.69</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>9.880000000000001</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>9.69</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>6.87</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>23.43</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>19.79</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>19.42</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>13.75</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>36.04</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>17.82</v>
       </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
       <c r="N6">
         <v>0</v>
       </c>
@@ -4456,47 +4549,50 @@
       <c r="R6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:18">
+      <c r="S6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
         <v>71.47</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>19.51</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>17.39</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>17.27</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>12.9</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>27.29</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>24.32</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>24.15</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>18.04</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>19.92</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>12.98</v>
       </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
       <c r="N7">
         <v>0</v>
       </c>
@@ -4507,52 +4603,55 @@
         <v>0</v>
       </c>
       <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
         <v>2471.77</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>49.69</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8">
         <v>104.62</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>18.24</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>15.66</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>15.52</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>11.07</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>17.43</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>14.96</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>14.83</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>10.58</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>14.61</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>9.32</v>
       </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
       <c r="N8">
         <v>0</v>
       </c>
@@ -4563,52 +4662,55 @@
         <v>0</v>
       </c>
       <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
         <v>13881.8</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>298.57</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9">
         <v>29.83</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>6.29</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>5.74</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>5.69</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>4.24</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>21.07</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>19.23</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>19.07</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>14.22</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>6.7</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>5.55</v>
       </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
       <c r="N9">
         <v>0</v>
       </c>
@@ -4619,52 +4721,55 @@
         <v>0</v>
       </c>
       <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
         <v>16292.67</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>194.51</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
         <v>37.15</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>7.33</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>6.78</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>6.76</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>5.02</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>19.74</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>18.23</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>18.19</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>13.51</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>7.35</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>6.04</v>
       </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
       <c r="N10">
         <v>0</v>
       </c>
@@ -4675,52 +4780,55 @@
         <v>0</v>
       </c>
       <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
         <v>12652</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>129.52</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11">
         <v>40.4</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>7.88</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>7.3</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>7.26</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>5.42</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>19.51</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>18.07</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>17.96</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>13.42</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>4.38</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>3.74</v>
       </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
       <c r="N11">
         <v>0</v>
       </c>
@@ -4731,9 +4839,12 @@
         <v>0</v>
       </c>
       <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
         <v>13912.34</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>125.98</v>
       </c>
     </row>

</xml_diff>